<commit_message>
Arreglando CSV muestra para ir acomodando los datos de Mario
</commit_message>
<xml_diff>
--- a/Proyectos/Mario_BisecciónTemporal/Datos_Sujeto3_Dummies.xlsx
+++ b/Proyectos/Mario_BisecciónTemporal/Datos_Sujeto3_Dummies.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Felisa\Proyectos\Mario_BisecciónTemporal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Proyectos\Mario_BisecciónTemporal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28200" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Datos_Sujeto3_Dummies" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="16">
   <si>
     <t>Condicion</t>
   </si>
@@ -53,19 +53,25 @@
     <t>M</t>
   </si>
   <si>
-    <t>Hits</t>
+    <t>Sujeto</t>
   </si>
   <si>
-    <t>Rechazos</t>
+    <t>Corto_enCorto</t>
   </si>
   <si>
-    <t>FA</t>
+    <t>Corto_enLargo</t>
   </si>
   <si>
-    <t>Signals</t>
+    <t>Largo_enCorto</t>
   </si>
   <si>
-    <t>Sujeto</t>
+    <t>Largo_enLargo</t>
+  </si>
+  <si>
+    <t>EnsayosCortos</t>
+  </si>
+  <si>
+    <t>EnsayosLargos</t>
   </si>
 </sst>
 </file>
@@ -383,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:J81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="J2" sqref="J2:J81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,11 +400,17 @@
     <col min="1" max="1" width="7.42578125" customWidth="1"/>
     <col min="2" max="2" width="7.28515625" customWidth="1"/>
     <col min="4" max="4" width="5.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
@@ -410,19 +422,25 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -439,16 +457,20 @@
         <v>54</v>
       </c>
       <c r="F2">
+        <v>28</v>
+      </c>
+      <c r="H2">
         <v>48</v>
       </c>
-      <c r="G2">
-        <v>28</v>
-      </c>
-      <c r="H2">
+      <c r="I2">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <f>F2+H2</f>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -465,16 +487,20 @@
         <v>44</v>
       </c>
       <c r="F3">
+        <v>35</v>
+      </c>
+      <c r="H3">
         <v>55</v>
       </c>
-      <c r="G3">
-        <v>35</v>
-      </c>
-      <c r="H3">
+      <c r="I3">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <f t="shared" ref="J3:J66" si="0">F3+H3</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -491,16 +517,20 @@
         <v>48</v>
       </c>
       <c r="F4">
+        <v>33</v>
+      </c>
+      <c r="H4">
         <v>47</v>
       </c>
-      <c r="G4">
-        <v>33</v>
-      </c>
-      <c r="H4">
+      <c r="I4">
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -517,16 +547,20 @@
         <v>45</v>
       </c>
       <c r="F5">
+        <v>29</v>
+      </c>
+      <c r="H5">
         <v>45</v>
       </c>
-      <c r="G5">
-        <v>29</v>
-      </c>
-      <c r="H5">
+      <c r="I5">
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -543,16 +577,20 @@
         <v>39</v>
       </c>
       <c r="F6">
+        <v>13</v>
+      </c>
+      <c r="H6">
         <v>33</v>
       </c>
-      <c r="G6">
-        <v>13</v>
-      </c>
-      <c r="H6">
+      <c r="I6">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -569,16 +607,20 @@
         <v>34</v>
       </c>
       <c r="F7">
+        <v>27</v>
+      </c>
+      <c r="H7">
         <v>35</v>
       </c>
-      <c r="G7">
-        <v>27</v>
-      </c>
-      <c r="H7">
+      <c r="I7">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -595,16 +637,20 @@
         <v>42</v>
       </c>
       <c r="F8">
+        <v>34</v>
+      </c>
+      <c r="H8">
         <v>44</v>
       </c>
-      <c r="G8">
-        <v>34</v>
-      </c>
-      <c r="H8">
+      <c r="I8">
         <v>47</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -621,16 +667,20 @@
         <v>50</v>
       </c>
       <c r="F9">
+        <v>32</v>
+      </c>
+      <c r="H9">
         <v>38</v>
       </c>
-      <c r="G9">
-        <v>32</v>
-      </c>
-      <c r="H9">
+      <c r="I9">
         <v>52</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -647,16 +697,20 @@
         <v>47</v>
       </c>
       <c r="F10">
+        <v>48</v>
+      </c>
+      <c r="H10">
         <v>54</v>
       </c>
-      <c r="G10">
-        <v>48</v>
-      </c>
-      <c r="H10">
+      <c r="I10">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -673,16 +727,20 @@
         <v>55</v>
       </c>
       <c r="F11">
+        <v>48</v>
+      </c>
+      <c r="H11">
         <v>56</v>
       </c>
-      <c r="G11">
-        <v>48</v>
-      </c>
-      <c r="H11">
+      <c r="I11">
         <v>59</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -699,16 +757,20 @@
         <v>43</v>
       </c>
       <c r="F12">
+        <v>30</v>
+      </c>
+      <c r="H12">
         <v>48</v>
       </c>
-      <c r="G12">
-        <v>30</v>
-      </c>
-      <c r="H12">
+      <c r="I12">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
@@ -725,16 +787,20 @@
         <v>39</v>
       </c>
       <c r="F13">
+        <v>18</v>
+      </c>
+      <c r="H13">
         <v>36</v>
       </c>
-      <c r="G13">
-        <v>18</v>
-      </c>
-      <c r="H13">
+      <c r="I13">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
@@ -751,16 +817,20 @@
         <v>33</v>
       </c>
       <c r="F14">
+        <v>19</v>
+      </c>
+      <c r="H14">
         <v>39</v>
       </c>
-      <c r="G14">
-        <v>19</v>
-      </c>
-      <c r="H14">
+      <c r="I14">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
@@ -777,16 +847,20 @@
         <v>49</v>
       </c>
       <c r="F15">
+        <v>29</v>
+      </c>
+      <c r="H15">
         <v>47</v>
       </c>
-      <c r="G15">
-        <v>29</v>
-      </c>
-      <c r="H15">
+      <c r="I15">
         <v>52</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -803,16 +877,20 @@
         <v>44</v>
       </c>
       <c r="F16">
+        <v>31</v>
+      </c>
+      <c r="H16">
         <v>47</v>
       </c>
-      <c r="G16">
-        <v>31</v>
-      </c>
-      <c r="H16">
+      <c r="I16">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -829,16 +907,20 @@
         <v>43</v>
       </c>
       <c r="F17">
+        <v>30</v>
+      </c>
+      <c r="H17">
         <v>48</v>
       </c>
-      <c r="G17">
-        <v>30</v>
-      </c>
-      <c r="H17">
+      <c r="I17">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -855,16 +937,20 @@
         <v>48</v>
       </c>
       <c r="F18">
+        <v>25</v>
+      </c>
+      <c r="H18">
         <v>27</v>
       </c>
-      <c r="G18">
-        <v>25</v>
-      </c>
-      <c r="H18">
+      <c r="I18">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3</v>
       </c>
@@ -881,16 +967,20 @@
         <v>51</v>
       </c>
       <c r="F19">
+        <v>31</v>
+      </c>
+      <c r="H19">
         <v>49</v>
       </c>
-      <c r="G19">
-        <v>31</v>
-      </c>
-      <c r="H19">
+      <c r="I19">
         <v>52</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -907,16 +997,20 @@
         <v>43</v>
       </c>
       <c r="F20">
+        <v>20</v>
+      </c>
+      <c r="H20">
         <v>38</v>
       </c>
-      <c r="G20">
-        <v>20</v>
-      </c>
-      <c r="H20">
+      <c r="I20">
         <v>44</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3</v>
       </c>
@@ -933,16 +1027,20 @@
         <v>35</v>
       </c>
       <c r="F21">
+        <v>18</v>
+      </c>
+      <c r="H21">
         <v>38</v>
       </c>
-      <c r="G21">
-        <v>18</v>
-      </c>
-      <c r="H21">
+      <c r="I21">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3</v>
       </c>
@@ -959,16 +1057,20 @@
         <v>43</v>
       </c>
       <c r="F22">
+        <v>20</v>
+      </c>
+      <c r="H22">
         <v>34</v>
       </c>
-      <c r="G22">
-        <v>20</v>
-      </c>
-      <c r="H22">
+      <c r="I22">
         <v>45</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3</v>
       </c>
@@ -985,16 +1087,20 @@
         <v>28</v>
       </c>
       <c r="F23">
+        <v>22</v>
+      </c>
+      <c r="H23">
         <v>36</v>
       </c>
-      <c r="G23">
-        <v>22</v>
-      </c>
-      <c r="H23">
+      <c r="I23">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1011,16 +1117,20 @@
         <v>23</v>
       </c>
       <c r="F24">
+        <v>16</v>
+      </c>
+      <c r="H24">
         <v>32</v>
       </c>
-      <c r="G24">
-        <v>16</v>
-      </c>
-      <c r="H24">
+      <c r="I24">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3</v>
       </c>
@@ -1037,16 +1147,20 @@
         <v>34</v>
       </c>
       <c r="F25">
+        <v>17</v>
+      </c>
+      <c r="H25">
         <v>31</v>
       </c>
-      <c r="G25">
-        <v>17</v>
-      </c>
-      <c r="H25">
+      <c r="I25">
         <v>34</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3</v>
       </c>
@@ -1063,16 +1177,20 @@
         <v>42</v>
       </c>
       <c r="F26">
+        <v>35</v>
+      </c>
+      <c r="H26">
         <v>41</v>
       </c>
-      <c r="G26">
-        <v>35</v>
-      </c>
-      <c r="H26">
+      <c r="I26">
         <v>46</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1089,16 +1207,20 @@
         <v>32</v>
       </c>
       <c r="F27">
+        <v>31</v>
+      </c>
+      <c r="H27">
         <v>39</v>
       </c>
-      <c r="G27">
-        <v>31</v>
-      </c>
-      <c r="H27">
+      <c r="I27">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1115,16 +1237,20 @@
         <v>34</v>
       </c>
       <c r="F28">
+        <v>24</v>
+      </c>
+      <c r="H28">
         <v>32</v>
       </c>
-      <c r="G28">
-        <v>24</v>
-      </c>
-      <c r="H28">
+      <c r="I28">
         <v>35</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3</v>
       </c>
@@ -1141,16 +1267,20 @@
         <v>33</v>
       </c>
       <c r="F29">
+        <v>18</v>
+      </c>
+      <c r="H29">
         <v>26</v>
       </c>
-      <c r="G29">
-        <v>18</v>
-      </c>
-      <c r="H29">
+      <c r="I29">
         <v>36</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1167,16 +1297,20 @@
         <v>34</v>
       </c>
       <c r="F30">
+        <v>36</v>
+      </c>
+      <c r="H30">
         <v>38</v>
       </c>
-      <c r="G30">
-        <v>36</v>
-      </c>
-      <c r="H30">
+      <c r="I30">
         <v>37</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1193,16 +1327,20 @@
         <v>31</v>
       </c>
       <c r="F31">
+        <v>19</v>
+      </c>
+      <c r="H31">
         <v>25</v>
       </c>
-      <c r="G31">
-        <v>19</v>
-      </c>
-      <c r="H31">
+      <c r="I31">
         <v>33</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J31">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1219,16 +1357,20 @@
         <v>29</v>
       </c>
       <c r="F32">
-        <v>32</v>
-      </c>
-      <c r="G32">
         <v>16</v>
       </c>
       <c r="H32">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>32</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1245,16 +1387,20 @@
         <v>43</v>
       </c>
       <c r="F33">
+        <v>25</v>
+      </c>
+      <c r="H33">
         <v>40</v>
       </c>
-      <c r="G33">
-        <v>25</v>
-      </c>
-      <c r="H33">
+      <c r="I33">
         <v>46</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J33">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1271,16 +1417,20 @@
         <v>31</v>
       </c>
       <c r="F34">
+        <v>22</v>
+      </c>
+      <c r="H34">
         <v>32</v>
       </c>
-      <c r="G34">
-        <v>22</v>
-      </c>
-      <c r="H34">
+      <c r="I34">
         <v>36</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J34">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3</v>
       </c>
@@ -1297,16 +1447,20 @@
         <v>31</v>
       </c>
       <c r="F35">
+        <v>23</v>
+      </c>
+      <c r="H35">
         <v>33</v>
       </c>
-      <c r="G35">
-        <v>23</v>
-      </c>
-      <c r="H35">
+      <c r="I35">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J35">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3</v>
       </c>
@@ -1325,14 +1479,18 @@
       <c r="F36">
         <v>15</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>15</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <v>28</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J36">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>3</v>
       </c>
@@ -1349,16 +1507,20 @@
         <v>33</v>
       </c>
       <c r="F37">
+        <v>24</v>
+      </c>
+      <c r="H37">
         <v>32</v>
       </c>
-      <c r="G37">
-        <v>24</v>
-      </c>
-      <c r="H37">
+      <c r="I37">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J37">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3</v>
       </c>
@@ -1375,16 +1537,20 @@
         <v>32</v>
       </c>
       <c r="F38">
+        <v>28</v>
+      </c>
+      <c r="H38">
         <v>34</v>
       </c>
-      <c r="G38">
-        <v>28</v>
-      </c>
-      <c r="H38">
+      <c r="I38">
         <v>33</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J38">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -1401,16 +1567,20 @@
         <v>24</v>
       </c>
       <c r="F39">
+        <v>12</v>
+      </c>
+      <c r="H39">
         <v>16</v>
       </c>
-      <c r="G39">
-        <v>12</v>
-      </c>
-      <c r="H39">
+      <c r="I39">
         <v>27</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J39">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3</v>
       </c>
@@ -1427,16 +1597,20 @@
         <v>29</v>
       </c>
       <c r="F40">
+        <v>27</v>
+      </c>
+      <c r="H40">
         <v>33</v>
       </c>
-      <c r="G40">
-        <v>27</v>
-      </c>
-      <c r="H40">
+      <c r="I40">
         <v>36</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J40">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>3</v>
       </c>
@@ -1453,16 +1627,20 @@
         <v>24</v>
       </c>
       <c r="F41">
+        <v>31</v>
+      </c>
+      <c r="H41">
         <v>35</v>
       </c>
-      <c r="G41">
-        <v>31</v>
-      </c>
-      <c r="H41">
+      <c r="I41">
         <v>30</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J41">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>3</v>
       </c>
@@ -1479,16 +1657,20 @@
         <v>37</v>
       </c>
       <c r="F42">
+        <v>22</v>
+      </c>
+      <c r="H42">
         <v>30</v>
       </c>
-      <c r="G42">
-        <v>22</v>
-      </c>
-      <c r="H42">
+      <c r="I42">
         <v>39</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J42">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>3</v>
       </c>
@@ -1505,16 +1687,20 @@
         <v>43</v>
       </c>
       <c r="F43">
+        <v>42</v>
+      </c>
+      <c r="H43">
         <v>50</v>
       </c>
-      <c r="G43">
-        <v>42</v>
-      </c>
-      <c r="H43">
+      <c r="I43">
         <v>45</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J43">
+        <f t="shared" si="0"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>3</v>
       </c>
@@ -1531,16 +1717,20 @@
         <v>38</v>
       </c>
       <c r="F44">
+        <v>25</v>
+      </c>
+      <c r="H44">
         <v>31</v>
       </c>
-      <c r="G44">
-        <v>25</v>
-      </c>
-      <c r="H44">
+      <c r="I44">
         <v>40</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J44">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3</v>
       </c>
@@ -1557,16 +1747,20 @@
         <v>41</v>
       </c>
       <c r="F45">
+        <v>36</v>
+      </c>
+      <c r="H45">
         <v>42</v>
       </c>
-      <c r="G45">
-        <v>36</v>
-      </c>
-      <c r="H45">
+      <c r="I45">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J45">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3</v>
       </c>
@@ -1583,16 +1777,20 @@
         <v>22</v>
       </c>
       <c r="F46">
+        <v>23</v>
+      </c>
+      <c r="H46">
         <v>29</v>
       </c>
-      <c r="G46">
+      <c r="I46">
         <v>23</v>
       </c>
-      <c r="H46">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J46">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3</v>
       </c>
@@ -1609,16 +1807,20 @@
         <v>33</v>
       </c>
       <c r="F47">
+        <v>16</v>
+      </c>
+      <c r="H47">
         <v>30</v>
       </c>
-      <c r="G47">
-        <v>16</v>
-      </c>
-      <c r="H47">
+      <c r="I47">
         <v>34</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J47">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3</v>
       </c>
@@ -1635,16 +1837,20 @@
         <v>37</v>
       </c>
       <c r="F48">
+        <v>15</v>
+      </c>
+      <c r="H48">
         <v>29</v>
       </c>
-      <c r="G48">
-        <v>15</v>
-      </c>
-      <c r="H48">
+      <c r="I48">
         <v>37</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J48">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>3</v>
       </c>
@@ -1661,16 +1867,20 @@
         <v>39</v>
       </c>
       <c r="F49">
+        <v>24</v>
+      </c>
+      <c r="H49">
         <v>38</v>
       </c>
-      <c r="G49">
-        <v>24</v>
-      </c>
-      <c r="H49">
+      <c r="I49">
         <v>40</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J49">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>3</v>
       </c>
@@ -1687,16 +1897,20 @@
         <v>38</v>
       </c>
       <c r="F50">
+        <v>25</v>
+      </c>
+      <c r="H50">
         <v>37</v>
       </c>
-      <c r="G50">
-        <v>25</v>
-      </c>
-      <c r="H50">
+      <c r="I50">
         <v>38</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J50">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>3</v>
       </c>
@@ -1713,16 +1927,20 @@
         <v>36</v>
       </c>
       <c r="F51">
+        <v>20</v>
+      </c>
+      <c r="H51">
         <v>34</v>
       </c>
-      <c r="G51">
-        <v>20</v>
-      </c>
-      <c r="H51">
+      <c r="I51">
         <v>38</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J51">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>3</v>
       </c>
@@ -1739,16 +1957,20 @@
         <v>52</v>
       </c>
       <c r="F52">
+        <v>38</v>
+      </c>
+      <c r="H52">
         <v>44</v>
       </c>
-      <c r="G52">
-        <v>38</v>
-      </c>
-      <c r="H52">
+      <c r="I52">
         <v>55</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J52">
+        <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>3</v>
       </c>
@@ -1765,16 +1987,20 @@
         <v>28</v>
       </c>
       <c r="F53">
+        <v>22</v>
+      </c>
+      <c r="H53">
         <v>30</v>
       </c>
-      <c r="G53">
-        <v>22</v>
-      </c>
-      <c r="H53">
+      <c r="I53">
         <v>28</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J53">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>3</v>
       </c>
@@ -1791,16 +2017,20 @@
         <v>44</v>
       </c>
       <c r="F54">
+        <v>34</v>
+      </c>
+      <c r="H54">
         <v>42</v>
       </c>
-      <c r="G54">
-        <v>34</v>
-      </c>
-      <c r="H54">
+      <c r="I54">
         <v>44</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J54">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>3</v>
       </c>
@@ -1817,16 +2047,20 @@
         <v>39</v>
       </c>
       <c r="F55">
+        <v>39</v>
+      </c>
+      <c r="H55">
         <v>45</v>
       </c>
-      <c r="G55">
-        <v>39</v>
-      </c>
-      <c r="H55">
+      <c r="I55">
         <v>41</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J55">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>3</v>
       </c>
@@ -1843,16 +2077,20 @@
         <v>44</v>
       </c>
       <c r="F56">
+        <v>38</v>
+      </c>
+      <c r="H56">
         <v>42</v>
       </c>
-      <c r="G56">
-        <v>38</v>
-      </c>
-      <c r="H56">
+      <c r="I56">
         <v>45</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J56">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>3</v>
       </c>
@@ -1869,16 +2107,20 @@
         <v>29</v>
       </c>
       <c r="F57">
+        <v>18</v>
+      </c>
+      <c r="H57">
         <v>34</v>
       </c>
-      <c r="G57">
-        <v>18</v>
-      </c>
-      <c r="H57">
+      <c r="I57">
         <v>33</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J57">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>3</v>
       </c>
@@ -1895,16 +2137,20 @@
         <v>29</v>
       </c>
       <c r="F58">
+        <v>16</v>
+      </c>
+      <c r="H58">
         <v>30</v>
       </c>
-      <c r="G58">
-        <v>16</v>
-      </c>
-      <c r="H58">
+      <c r="I58">
         <v>33</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J58">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>3</v>
       </c>
@@ -1921,16 +2167,20 @@
         <v>32</v>
       </c>
       <c r="F59">
+        <v>22</v>
+      </c>
+      <c r="H59">
         <v>34</v>
       </c>
-      <c r="G59">
-        <v>22</v>
-      </c>
-      <c r="H59">
+      <c r="I59">
         <v>33</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J59">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>3</v>
       </c>
@@ -1947,16 +2197,20 @@
         <v>34</v>
       </c>
       <c r="F60">
+        <v>12</v>
+      </c>
+      <c r="H60">
         <v>28</v>
       </c>
-      <c r="G60">
-        <v>12</v>
-      </c>
-      <c r="H60">
+      <c r="I60">
         <v>36</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J60">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>3</v>
       </c>
@@ -1973,16 +2227,20 @@
         <v>27</v>
       </c>
       <c r="F61">
+        <v>15</v>
+      </c>
+      <c r="H61">
         <v>31</v>
       </c>
-      <c r="G61">
-        <v>15</v>
-      </c>
-      <c r="H61">
+      <c r="I61">
         <v>30</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J61">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>3</v>
       </c>
@@ -2001,14 +2259,18 @@
       <c r="F62">
         <v>34</v>
       </c>
-      <c r="G62">
+      <c r="H62">
         <v>34</v>
       </c>
-      <c r="H62">
+      <c r="I62">
         <v>37</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J62">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>3</v>
       </c>
@@ -2025,16 +2287,20 @@
         <v>39</v>
       </c>
       <c r="F63">
+        <v>29</v>
+      </c>
+      <c r="H63">
         <v>31</v>
       </c>
-      <c r="G63">
-        <v>29</v>
-      </c>
-      <c r="H63">
+      <c r="I63">
         <v>42</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J63">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>3</v>
       </c>
@@ -2051,16 +2317,20 @@
         <v>34</v>
       </c>
       <c r="F64">
+        <v>30</v>
+      </c>
+      <c r="H64">
         <v>34</v>
       </c>
-      <c r="G64">
-        <v>30</v>
-      </c>
-      <c r="H64">
+      <c r="I64">
         <v>36</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J64">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>3</v>
       </c>
@@ -2077,16 +2347,20 @@
         <v>25</v>
       </c>
       <c r="F65">
+        <v>19</v>
+      </c>
+      <c r="H65">
         <v>21</v>
       </c>
-      <c r="G65">
-        <v>19</v>
-      </c>
-      <c r="H65">
+      <c r="I65">
         <v>27</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J65">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>3</v>
       </c>
@@ -2103,16 +2377,20 @@
         <v>23</v>
       </c>
       <c r="F66">
+        <v>14</v>
+      </c>
+      <c r="H66">
         <v>20</v>
       </c>
-      <c r="G66">
-        <v>14</v>
-      </c>
-      <c r="H66">
+      <c r="I66">
         <v>27</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J66">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>3</v>
       </c>
@@ -2129,16 +2407,20 @@
         <v>45</v>
       </c>
       <c r="F67">
+        <v>29</v>
+      </c>
+      <c r="H67">
         <v>41</v>
       </c>
-      <c r="G67">
-        <v>29</v>
-      </c>
-      <c r="H67">
+      <c r="I67">
         <v>47</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J67">
+        <f t="shared" ref="J67:J81" si="1">F67+H67</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>3</v>
       </c>
@@ -2155,16 +2437,20 @@
         <v>35</v>
       </c>
       <c r="F68">
-        <v>35</v>
-      </c>
-      <c r="G68">
         <v>25</v>
       </c>
       <c r="H68">
         <v>35</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68">
+        <v>35</v>
+      </c>
+      <c r="J68">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>3</v>
       </c>
@@ -2181,16 +2467,20 @@
         <v>40</v>
       </c>
       <c r="F69">
+        <v>29</v>
+      </c>
+      <c r="H69">
         <v>33</v>
       </c>
-      <c r="G69">
-        <v>29</v>
-      </c>
-      <c r="H69">
+      <c r="I69">
         <v>41</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J69">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>3</v>
       </c>
@@ -2207,16 +2497,20 @@
         <v>38</v>
       </c>
       <c r="F70">
+        <v>36</v>
+      </c>
+      <c r="H70">
         <v>40</v>
       </c>
-      <c r="G70">
-        <v>36</v>
-      </c>
-      <c r="H70">
+      <c r="I70">
         <v>39</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J70">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>3</v>
       </c>
@@ -2233,16 +2527,20 @@
         <v>31</v>
       </c>
       <c r="F71">
+        <v>24</v>
+      </c>
+      <c r="H71">
         <v>32</v>
       </c>
-      <c r="G71">
-        <v>24</v>
-      </c>
-      <c r="H71">
+      <c r="I71">
         <v>35</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J71">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>3</v>
       </c>
@@ -2259,16 +2557,20 @@
         <v>35</v>
       </c>
       <c r="F72">
+        <v>33</v>
+      </c>
+      <c r="H72">
         <v>39</v>
       </c>
-      <c r="G72">
-        <v>33</v>
-      </c>
-      <c r="H72">
+      <c r="I72">
         <v>37</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J72">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>3</v>
       </c>
@@ -2285,16 +2587,20 @@
         <v>39</v>
       </c>
       <c r="F73">
+        <v>40</v>
+      </c>
+      <c r="H73">
         <v>44</v>
       </c>
-      <c r="G73">
-        <v>40</v>
-      </c>
-      <c r="H73">
+      <c r="I73">
         <v>45</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J73">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>3</v>
       </c>
@@ -2311,16 +2617,20 @@
         <v>39</v>
       </c>
       <c r="F74">
+        <v>41</v>
+      </c>
+      <c r="H74">
         <v>45</v>
       </c>
-      <c r="G74">
-        <v>41</v>
-      </c>
-      <c r="H74">
+      <c r="I74">
         <v>42</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J74">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>3</v>
       </c>
@@ -2337,16 +2647,20 @@
         <v>29</v>
       </c>
       <c r="F75">
+        <v>22</v>
+      </c>
+      <c r="H75">
         <v>26</v>
       </c>
-      <c r="G75">
-        <v>22</v>
-      </c>
-      <c r="H75">
+      <c r="I75">
         <v>32</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J75">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>3</v>
       </c>
@@ -2363,16 +2677,20 @@
         <v>36</v>
       </c>
       <c r="F76">
+        <v>41</v>
+      </c>
+      <c r="H76">
         <v>49</v>
       </c>
-      <c r="G76">
-        <v>41</v>
-      </c>
-      <c r="H76">
+      <c r="I76">
         <v>37</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J76">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>3</v>
       </c>
@@ -2389,16 +2707,20 @@
         <v>43</v>
       </c>
       <c r="F77">
-        <v>53</v>
-      </c>
-      <c r="G77">
         <v>42</v>
       </c>
       <c r="H77">
         <v>53</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77">
+        <v>53</v>
+      </c>
+      <c r="J77">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>3</v>
       </c>
@@ -2415,16 +2737,20 @@
         <v>41</v>
       </c>
       <c r="F78">
+        <v>25</v>
+      </c>
+      <c r="H78">
         <v>39</v>
       </c>
-      <c r="G78">
-        <v>25</v>
-      </c>
-      <c r="H78">
+      <c r="I78">
         <v>45</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J78">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>3</v>
       </c>
@@ -2441,16 +2767,20 @@
         <v>31</v>
       </c>
       <c r="F79">
+        <v>21</v>
+      </c>
+      <c r="H79">
         <v>25</v>
       </c>
-      <c r="G79">
-        <v>21</v>
-      </c>
-      <c r="H79">
+      <c r="I79">
         <v>36</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J79">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>3</v>
       </c>
@@ -2467,16 +2797,20 @@
         <v>28</v>
       </c>
       <c r="F80">
+        <v>23</v>
+      </c>
+      <c r="H80">
         <v>33</v>
       </c>
-      <c r="G80">
-        <v>23</v>
-      </c>
-      <c r="H80">
+      <c r="I80">
         <v>35</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J80">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>3</v>
       </c>
@@ -2493,13 +2827,17 @@
         <v>25</v>
       </c>
       <c r="F81">
+        <v>24</v>
+      </c>
+      <c r="H81">
         <v>36</v>
       </c>
-      <c r="G81">
-        <v>24</v>
-      </c>
-      <c r="H81">
+      <c r="I81">
         <v>27</v>
+      </c>
+      <c r="J81">
+        <f t="shared" si="1"/>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>